<commit_message>
feat: udistrital/sga_cliente#1339 reportes horario y general PTD
- Se desarrolla la funcionalidad para graficar el horario del docente segun carga lectiva o actividades o ambos
  - Incluye ajuste segun rango de horas si no se usa todo el horario, esto con el fin de agrandar las celdas para mejor visualización
- Se crea controlador de reporte verificacion cumplimiento, por el momento está en blanco
</commit_message>
<xml_diff>
--- a/static/templates/PTD.xlsx
+++ b/static/templates/PTD.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NeFa\Downloads\Telegram Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F7DEB1-0195-447F-99EE-65553896D8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24921BE0-6C0F-4DE6-BA16-2BEC2D6DF020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{20552BE1-5C54-4987-806D-333FCE08028B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Carga_Lectiva_PTD" sheetId="1" r:id="rId1"/>
+    <sheet name="PTD" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -539,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -646,8 +646,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -983,7 +986,7 @@
   <dimension ref="A2:AO102"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+      <selection activeCell="B5" sqref="B5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,55 +1330,55 @@
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="57" t="s">
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="57" t="s">
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="57" t="s">
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="57" t="s">
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="59"/>
+      <c r="AA12" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="57"/>
-      <c r="AD12" s="57"/>
-      <c r="AE12" s="58"/>
-      <c r="AF12" s="57" t="s">
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="59"/>
+      <c r="AF12" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AG12" s="57"/>
-      <c r="AH12" s="57"/>
-      <c r="AI12" s="57"/>
-      <c r="AJ12" s="58"/>
-      <c r="AK12" s="57" t="s">
+      <c r="AG12" s="58"/>
+      <c r="AH12" s="58"/>
+      <c r="AI12" s="58"/>
+      <c r="AJ12" s="59"/>
+      <c r="AK12" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AL12" s="57"/>
-      <c r="AM12" s="57"/>
-      <c r="AN12" s="57"/>
-      <c r="AO12" s="60"/>
+      <c r="AL12" s="58"/>
+      <c r="AM12" s="58"/>
+      <c r="AN12" s="58"/>
+      <c r="AO12" s="61"/>
     </row>
     <row r="13" spans="1:41" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
@@ -4692,131 +4695,131 @@
     </row>
     <row r="93" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A93" s="29"/>
-      <c r="B93" s="54"/>
-      <c r="C93" s="54"/>
-      <c r="D93" s="54"/>
-      <c r="E93" s="54"/>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="54"/>
-      <c r="I93" s="54"/>
-      <c r="J93" s="54"/>
-      <c r="K93" s="54"/>
-      <c r="L93" s="54"/>
-      <c r="M93" s="54"/>
-      <c r="N93" s="54"/>
-      <c r="O93" s="54"/>
-      <c r="P93" s="54"/>
-      <c r="Q93" s="54"/>
-      <c r="R93" s="54"/>
-      <c r="S93" s="54"/>
-      <c r="T93" s="54"/>
-      <c r="U93" s="54"/>
-      <c r="V93" s="54"/>
-      <c r="W93" s="54"/>
-      <c r="X93" s="54"/>
-      <c r="Y93" s="54"/>
-      <c r="Z93" s="54"/>
-      <c r="AA93" s="54"/>
-      <c r="AB93" s="54"/>
-      <c r="AC93" s="54"/>
-      <c r="AD93" s="54"/>
-      <c r="AE93" s="54"/>
-      <c r="AF93" s="54"/>
-      <c r="AG93" s="54"/>
-      <c r="AH93" s="54"/>
-      <c r="AI93" s="54"/>
-      <c r="AJ93" s="54"/>
-      <c r="AK93" s="54"/>
-      <c r="AL93" s="54"/>
-      <c r="AM93" s="54"/>
-      <c r="AN93" s="54"/>
+      <c r="B93" s="56"/>
+      <c r="C93" s="56"/>
+      <c r="D93" s="56"/>
+      <c r="E93" s="56"/>
+      <c r="F93" s="56"/>
+      <c r="G93" s="56"/>
+      <c r="H93" s="56"/>
+      <c r="I93" s="56"/>
+      <c r="J93" s="56"/>
+      <c r="K93" s="56"/>
+      <c r="L93" s="56"/>
+      <c r="M93" s="56"/>
+      <c r="N93" s="56"/>
+      <c r="O93" s="56"/>
+      <c r="P93" s="56"/>
+      <c r="Q93" s="56"/>
+      <c r="R93" s="56"/>
+      <c r="S93" s="56"/>
+      <c r="T93" s="56"/>
+      <c r="U93" s="56"/>
+      <c r="V93" s="56"/>
+      <c r="W93" s="56"/>
+      <c r="X93" s="56"/>
+      <c r="Y93" s="56"/>
+      <c r="Z93" s="56"/>
+      <c r="AA93" s="56"/>
+      <c r="AB93" s="56"/>
+      <c r="AC93" s="56"/>
+      <c r="AD93" s="56"/>
+      <c r="AE93" s="56"/>
+      <c r="AF93" s="56"/>
+      <c r="AG93" s="56"/>
+      <c r="AH93" s="56"/>
+      <c r="AI93" s="56"/>
+      <c r="AJ93" s="56"/>
+      <c r="AK93" s="56"/>
+      <c r="AL93" s="56"/>
+      <c r="AM93" s="56"/>
+      <c r="AN93" s="56"/>
       <c r="AO93" s="20"/>
     </row>
     <row r="94" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A94" s="29"/>
-      <c r="B94" s="56"/>
-      <c r="C94" s="56"/>
-      <c r="D94" s="56"/>
-      <c r="E94" s="56"/>
-      <c r="F94" s="56"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="56"/>
-      <c r="I94" s="56"/>
-      <c r="J94" s="56"/>
-      <c r="K94" s="56"/>
-      <c r="L94" s="56"/>
-      <c r="M94" s="56"/>
-      <c r="N94" s="56"/>
-      <c r="O94" s="56"/>
-      <c r="P94" s="56"/>
-      <c r="Q94" s="56"/>
-      <c r="R94" s="56"/>
-      <c r="S94" s="56"/>
-      <c r="T94" s="56"/>
-      <c r="U94" s="56"/>
-      <c r="V94" s="56"/>
-      <c r="W94" s="56"/>
-      <c r="X94" s="56"/>
-      <c r="Y94" s="56"/>
-      <c r="Z94" s="56"/>
-      <c r="AA94" s="56"/>
-      <c r="AB94" s="56"/>
-      <c r="AC94" s="56"/>
-      <c r="AD94" s="56"/>
-      <c r="AE94" s="56"/>
-      <c r="AF94" s="56"/>
-      <c r="AG94" s="56"/>
-      <c r="AH94" s="56"/>
-      <c r="AI94" s="56"/>
-      <c r="AJ94" s="56"/>
-      <c r="AK94" s="56"/>
-      <c r="AL94" s="56"/>
-      <c r="AM94" s="56"/>
-      <c r="AN94" s="56"/>
+      <c r="B94" s="57"/>
+      <c r="C94" s="57"/>
+      <c r="D94" s="57"/>
+      <c r="E94" s="57"/>
+      <c r="F94" s="57"/>
+      <c r="G94" s="57"/>
+      <c r="H94" s="57"/>
+      <c r="I94" s="57"/>
+      <c r="J94" s="57"/>
+      <c r="K94" s="57"/>
+      <c r="L94" s="57"/>
+      <c r="M94" s="57"/>
+      <c r="N94" s="57"/>
+      <c r="O94" s="57"/>
+      <c r="P94" s="57"/>
+      <c r="Q94" s="57"/>
+      <c r="R94" s="57"/>
+      <c r="S94" s="57"/>
+      <c r="T94" s="57"/>
+      <c r="U94" s="57"/>
+      <c r="V94" s="57"/>
+      <c r="W94" s="57"/>
+      <c r="X94" s="57"/>
+      <c r="Y94" s="57"/>
+      <c r="Z94" s="57"/>
+      <c r="AA94" s="57"/>
+      <c r="AB94" s="57"/>
+      <c r="AC94" s="57"/>
+      <c r="AD94" s="57"/>
+      <c r="AE94" s="57"/>
+      <c r="AF94" s="57"/>
+      <c r="AG94" s="57"/>
+      <c r="AH94" s="57"/>
+      <c r="AI94" s="57"/>
+      <c r="AJ94" s="57"/>
+      <c r="AK94" s="57"/>
+      <c r="AL94" s="57"/>
+      <c r="AM94" s="57"/>
+      <c r="AN94" s="57"/>
       <c r="AO94" s="20"/>
     </row>
     <row r="95" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="56"/>
-      <c r="C95" s="56"/>
-      <c r="D95" s="56"/>
-      <c r="E95" s="56"/>
-      <c r="F95" s="56"/>
-      <c r="G95" s="56"/>
-      <c r="H95" s="56"/>
-      <c r="I95" s="56"/>
-      <c r="J95" s="56"/>
-      <c r="K95" s="56"/>
-      <c r="L95" s="56"/>
-      <c r="M95" s="56"/>
-      <c r="N95" s="56"/>
-      <c r="O95" s="56"/>
-      <c r="P95" s="56"/>
-      <c r="Q95" s="56"/>
-      <c r="R95" s="56"/>
-      <c r="S95" s="56"/>
-      <c r="T95" s="56"/>
-      <c r="U95" s="56"/>
-      <c r="V95" s="56"/>
-      <c r="W95" s="56"/>
-      <c r="X95" s="56"/>
-      <c r="Y95" s="56"/>
-      <c r="Z95" s="56"/>
-      <c r="AA95" s="56"/>
-      <c r="AB95" s="56"/>
-      <c r="AC95" s="56"/>
-      <c r="AD95" s="56"/>
-      <c r="AE95" s="56"/>
-      <c r="AF95" s="56"/>
-      <c r="AG95" s="56"/>
-      <c r="AH95" s="56"/>
-      <c r="AI95" s="56"/>
-      <c r="AJ95" s="56"/>
-      <c r="AK95" s="56"/>
-      <c r="AL95" s="56"/>
-      <c r="AM95" s="56"/>
-      <c r="AN95" s="56"/>
+      <c r="B95" s="57"/>
+      <c r="C95" s="57"/>
+      <c r="D95" s="57"/>
+      <c r="E95" s="57"/>
+      <c r="F95" s="57"/>
+      <c r="G95" s="57"/>
+      <c r="H95" s="57"/>
+      <c r="I95" s="57"/>
+      <c r="J95" s="57"/>
+      <c r="K95" s="57"/>
+      <c r="L95" s="57"/>
+      <c r="M95" s="57"/>
+      <c r="N95" s="57"/>
+      <c r="O95" s="57"/>
+      <c r="P95" s="57"/>
+      <c r="Q95" s="57"/>
+      <c r="R95" s="57"/>
+      <c r="S95" s="57"/>
+      <c r="T95" s="57"/>
+      <c r="U95" s="57"/>
+      <c r="V95" s="57"/>
+      <c r="W95" s="57"/>
+      <c r="X95" s="57"/>
+      <c r="Y95" s="57"/>
+      <c r="Z95" s="57"/>
+      <c r="AA95" s="57"/>
+      <c r="AB95" s="57"/>
+      <c r="AC95" s="57"/>
+      <c r="AD95" s="57"/>
+      <c r="AE95" s="57"/>
+      <c r="AF95" s="57"/>
+      <c r="AG95" s="57"/>
+      <c r="AH95" s="57"/>
+      <c r="AI95" s="57"/>
+      <c r="AJ95" s="57"/>
+      <c r="AK95" s="57"/>
+      <c r="AL95" s="57"/>
+      <c r="AM95" s="57"/>
+      <c r="AN95" s="57"/>
       <c r="AO95" s="20"/>
     </row>
     <row r="96" spans="1:41" x14ac:dyDescent="0.25">

</xml_diff>